<commit_message>
Completed Test Case 3 : User should be able to populate ToDos with Chines Characters
</commit_message>
<xml_diff>
--- a/src/test/resources/BS_Data_VUE.xlsx
+++ b/src/test/resources/BS_Data_VUE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\Vic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\IdeaProjects\VueChecker\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1712966-CDFA-4F92-94CB-DF495B6D2147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014774EF-1910-400E-A744-B39CF2F4F48F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10080" xr2:uid="{5A1B083B-37B4-4FA6-8309-DA41FD67F6CD}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7100" xr2:uid="{5A1B083B-37B4-4FA6-8309-DA41FD67F6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="BS_DATA_VUE" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>ContextID</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>NIL</t>
-  </si>
-  <si>
-    <t>VUE_003_UserShouldNotBeAbleToWriteMoreThan20CharsLong</t>
   </si>
   <si>
     <t>Positive</t>
@@ -122,6 +119,15 @@
   </si>
   <si>
     <t>I need to wake up at 6.30am | I need to brush my teeth</t>
+  </si>
+  <si>
+    <t>VUE_003_UserShouldBeAbleToPopulateToDosWithChinese</t>
+  </si>
+  <si>
+    <t>我需要在早上6.30醒來 | 我需要刷牙</t>
+  </si>
+  <si>
+    <t>VUE_004_UserShouldNotBeAbleToWriteMoreThan20CharsLong</t>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -256,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,13 +585,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174C7D57-E917-4B51-9557-9FFC2E82BD38}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -616,48 +625,67 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -689,39 +717,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="4"/>
     </row>

</xml_diff>

<commit_message>
Completed All Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/BS_Data_VUE.xlsx
+++ b/src/test/resources/BS_Data_VUE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\IdeaProjects\VueChecker\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014774EF-1910-400E-A744-B39CF2F4F48F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC578F0-00B0-482D-BC33-A580B166B005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7100" xr2:uid="{5A1B083B-37B4-4FA6-8309-DA41FD67F6CD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10080" xr2:uid="{5A1B083B-37B4-4FA6-8309-DA41FD67F6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="BS_DATA_VUE" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>ContextID</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>ScenarioType</t>
-  </si>
-  <si>
-    <t>VUE_001_UserShouldBeAbleToPopulateToDos</t>
-  </si>
-  <si>
-    <t>VUE_002_UserShouldBeAbleToDeleteToDos</t>
   </si>
   <si>
     <t>DependentVariable</t>
@@ -121,13 +115,34 @@
     <t>I need to wake up at 6.30am | I need to brush my teeth</t>
   </si>
   <si>
-    <t>VUE_003_UserShouldBeAbleToPopulateToDosWithChinese</t>
-  </si>
-  <si>
     <t>我需要在早上6.30醒來 | 我需要刷牙</t>
   </si>
   <si>
-    <t>VUE_004_UserShouldNotBeAbleToWriteMoreThan20CharsLong</t>
+    <t>VUE001_UserShouldBeAbleToPopulateToDos</t>
+  </si>
+  <si>
+    <t>VUE002_UserShouldBeAbleToDeleteToDos</t>
+  </si>
+  <si>
+    <t>VUE003_UserShouldBeAbleToPopulateToDosWithChinese</t>
+  </si>
+  <si>
+    <t>VUE004_UserShouldNotBeAbleToWriteMoreThan20CharsLong</t>
+  </si>
+  <si>
+    <t>ListOfCompletedItems</t>
+  </si>
+  <si>
+    <t>I need to wake up at 6.30am</t>
+  </si>
+  <si>
+    <t>Out Of Scope</t>
+  </si>
+  <si>
+    <t>VUE004_UserShouldBeAbleToFindCompletedTaskAtCompletedPage</t>
+  </si>
+  <si>
+    <t>ListOfToBeDeletedItems</t>
   </si>
 </sst>
 </file>
@@ -244,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -266,6 +281,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,13 +602,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174C7D57-E917-4B51-9557-9FFC2E82BD38}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,92 +618,156 @@
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="39.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="25.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,39 +798,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4"/>
     </row>

</xml_diff>